<commit_message>
fix: txt file charset and new xlsx example
</commit_message>
<xml_diff>
--- a/packages/frontend/public/example.xlsx
+++ b/packages/frontend/public/example.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusflopes\github\xls2dom\packages\frontend\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B3A13F-5282-4D7A-8460-D06D2426C732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="13660" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Data</t>
   </si>
@@ -39,25 +45,43 @@
     <t>Historico</t>
   </si>
   <si>
-    <t>Pagamento de fornecedor conf. comprovante.</t>
-  </si>
-  <si>
-    <t>Pagamento de cliente</t>
-  </si>
-  <si>
-    <t>Depósito em Cheque</t>
-  </si>
-  <si>
-    <t>Saque para o Caixa</t>
-  </si>
-  <si>
-    <t>Recebimento de Venda</t>
+    <t>Pagamento de despesa de material de escritório conf.  Caixa.</t>
+  </si>
+  <si>
+    <t>Pagamento de despesa de material de escritório conf.  Banco.</t>
+  </si>
+  <si>
+    <t>Venda de mercadoria a prazo.</t>
+  </si>
+  <si>
+    <t>CMV debitado estoque ref. Venda.</t>
+  </si>
+  <si>
+    <t>Vendo de mercadoria a  vista com  pagamento por TED.</t>
+  </si>
+  <si>
+    <t>Prestação de serviços a cliente com pagamento à prazo.</t>
+  </si>
+  <si>
+    <t>Pagamento Custo dos Serviços pretados conf. Banco.</t>
+  </si>
+  <si>
+    <t>Pagamento Custo dos Serviços pretados conf. Caixa.</t>
+  </si>
+  <si>
+    <t>Custo dos Serviços pretados contratados com Fornecedor para 30 dias.</t>
+  </si>
+  <si>
+    <t>Pagamento de fornecedor conf. Transferência bancária.</t>
+  </si>
+  <si>
+    <t>Recebimento de valores de cliente.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$-416]\ #,##0.00;[Red]\-[$R$-416]\ #,##0.00"/>
   </numFmts>
@@ -99,6 +123,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,23 +455,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="1"/>
-    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,15 +488,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>500</v>
@@ -473,327 +505,395 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43467</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>359</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
         <v>350</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43468</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>519</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>408</v>
       </c>
       <c r="D4" s="1">
         <v>450</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43469</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>464</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1">
         <v>153</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43470</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>408</v>
       </c>
       <c r="D6" s="1">
         <v>215</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43471</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>464</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D7" s="1">
         <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43472</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>519</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>411</v>
       </c>
       <c r="D8" s="1">
         <v>542</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43473</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>467</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D9" s="1">
         <v>456</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43474</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>467</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="1">
         <v>954</v>
       </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43475</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>467</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>506</v>
       </c>
       <c r="D11" s="1">
         <v>500</v>
       </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43476</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>506</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1">
         <v>350</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43477</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>519</v>
       </c>
       <c r="D13" s="1">
         <v>450</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43478</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
-        <v>153</v>
+        <v>500</v>
       </c>
       <c r="E14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43479</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>359</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>215</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>350</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43480</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>519</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>408</v>
       </c>
       <c r="D16" s="1">
-        <v>34</v>
+        <v>450</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43481</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>464</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D17" s="1">
-        <v>542</v>
+        <v>153</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43482</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>408</v>
       </c>
       <c r="D18" s="1">
-        <v>456</v>
+        <v>215</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43483</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>464</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="D19" s="1">
-        <v>954</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43484</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>519</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>411</v>
       </c>
       <c r="D20" s="1">
-        <v>153</v>
+        <v>542</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43485</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>467</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D21" s="1">
-        <v>154</v>
+        <v>456</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>43486</v>
+      </c>
+      <c r="B22">
+        <v>467</v>
+      </c>
+      <c r="C22">
         <v>5</v>
+      </c>
+      <c r="D22" s="1">
+        <v>954</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>43487</v>
+      </c>
+      <c r="B23">
+        <v>467</v>
+      </c>
+      <c r="C23">
+        <v>506</v>
+      </c>
+      <c r="D23" s="1">
+        <v>500</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>43488</v>
+      </c>
+      <c r="B24">
+        <v>506</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" s="1">
+        <v>350</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>43489</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>519</v>
+      </c>
+      <c r="D25" s="1">
+        <v>450</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: fixed example.xlsx and README
</commit_message>
<xml_diff>
--- a/packages/frontend/public/example.xlsx
+++ b/packages/frontend/public/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusflopes\github\xls2dom\packages\frontend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B3A13F-5282-4D7A-8460-D06D2426C732}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE943D3-6A82-4DB0-863F-DC17099790A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16515" yWindow="1800" windowWidth="14430" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -468,7 +468,7 @@
     <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="62" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>